<commit_message>
Actualzacion con reportes corregidos
</commit_message>
<xml_diff>
--- a/modules/Equipo/reports/Custodio.xlsx
+++ b/modules/Equipo/reports/Custodio.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Inventario\modules\Equipo\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Inventario2.0\modules\Equipo\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433DE07C-4583-4864-806E-5EC073EAD088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64649D8-F5ED-4ECE-B9A0-8071597308AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FD87A278-38B4-4659-9D16-AC62AB542BB6}"/>
   </bookViews>
@@ -90,9 +90,6 @@
     <t>Modelo:</t>
   </si>
   <si>
-    <t>Estado:</t>
-  </si>
-  <si>
     <t>Valor del Equipo:</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>Entregado por</t>
+  </si>
+  <si>
+    <t>Proyecto:</t>
   </si>
 </sst>
 </file>
@@ -354,7 +354,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -396,14 +396,49 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -414,10 +449,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -425,52 +456,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -810,8 +803,8 @@
   </sheetPr>
   <dimension ref="A1:W52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A26" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -857,69 +850,69 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
       <c r="J7" s="1"/>
       <c r="K7" s="2"/>
     </row>
@@ -966,15 +959,15 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="23"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="23"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
         <v>4</v>
@@ -987,27 +980,27 @@
     </row>
     <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="43"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
       <c r="J12" s="3"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
       <c r="J13" s="3"/>
       <c r="K13" s="2"/>
     </row>
@@ -1026,51 +1019,51 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="25"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="23"/>
+      <c r="F15" s="25"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
       <c r="J16" s="3"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:23" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
       <c r="J17" s="3"/>
       <c r="K17" s="2"/>
-      <c r="N17" s="44"/>
+      <c r="N17" s="23"/>
     </row>
     <row r="18" spans="1:23" ht="10.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
@@ -1138,16 +1131,16 @@
       <c r="I22" s="11"/>
       <c r="J22" s="6"/>
       <c r="K22" s="2"/>
-      <c r="N22" s="40"/>
-      <c r="O22" s="40"/>
-      <c r="P22" s="40"/>
-      <c r="Q22" s="40"/>
-      <c r="R22" s="40"/>
-      <c r="S22" s="31"/>
-      <c r="T22" s="31"/>
-      <c r="U22" s="31"/>
-      <c r="V22" s="31"/>
-      <c r="W22" s="31"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="34"/>
+      <c r="Q22" s="34"/>
+      <c r="R22" s="34"/>
+      <c r="S22" s="24"/>
+      <c r="T22" s="24"/>
+      <c r="U22" s="24"/>
+      <c r="V22" s="24"/>
+      <c r="W22" s="24"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
@@ -1161,40 +1154,41 @@
       <c r="I23" s="1"/>
       <c r="J23" s="3"/>
       <c r="K23" s="2"/>
-      <c r="N23" s="40"/>
-      <c r="O23" s="40"/>
-      <c r="P23" s="40"/>
-      <c r="Q23" s="40"/>
-      <c r="R23" s="40"/>
-      <c r="S23" s="31"/>
-      <c r="T23" s="31"/>
-      <c r="U23" s="31"/>
-      <c r="V23" s="31"/>
-      <c r="W23" s="31"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="34"/>
+      <c r="Q23" s="34"/>
+      <c r="R23" s="34"/>
+      <c r="S23" s="24"/>
+      <c r="T23" s="24"/>
+      <c r="U23" s="24"/>
+      <c r="V23" s="24"/>
+      <c r="W23" s="24"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="28"/>
-      <c r="F24" t="s">
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="1"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
       <c r="J24" s="3"/>
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:23" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
-      <c r="B25" s="1"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="F25" s="16"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -1203,53 +1197,54 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="F26" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="1"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
       <c r="J26" s="3"/>
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
-      <c r="B27" s="1"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="F27" s="16"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="3"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:23" ht="16.899999999999999" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="1"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
       <c r="J28" s="3"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:23" ht="16.899999999999999" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
-      <c r="B29" s="1"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="21"/>
       <c r="D29" s="21"/>
       <c r="E29" s="1"/>
@@ -1262,35 +1257,35 @@
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
-      <c r="B30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="1"/>
+      <c r="B30" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
       <c r="J30" s="3"/>
       <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="1"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
       <c r="J31" s="3"/>
       <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
-      <c r="B32" s="1"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="21"/>
       <c r="D32" s="21"/>
       <c r="E32" s="1"/>
@@ -1300,37 +1295,36 @@
       <c r="I32" s="1"/>
       <c r="J32" s="3"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="45"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
-      <c r="B33" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="35"/>
-      <c r="I33" s="1"/>
+      <c r="B33" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
       <c r="J33" s="3"/>
       <c r="K33" s="2"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="1"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
       <c r="J34" s="3"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="8"/>
       <c r="B35" s="9"/>
       <c r="C35" s="22"/>
@@ -1343,7 +1337,7 @@
       <c r="J35" s="10"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="16.899999999999999" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="21"/>
@@ -1359,7 +1353,7 @@
     <row r="37" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1372,18 +1366,18 @@
       <c r="K37" s="2"/>
     </row>
     <row r="38" spans="1:11" ht="154.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="37"/>
-      <c r="J38" s="38"/>
+      <c r="A38" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="33"/>
       <c r="K38" s="2"/>
     </row>
     <row r="39" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1455,12 +1449,12 @@
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -1472,12 +1466,12 @@
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="1"/>
       <c r="F45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G45" s="20"/>
       <c r="H45" s="20"/>
@@ -1540,8 +1534,8 @@
     <row r="51" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -1556,35 +1550,33 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="24">
-    <mergeCell ref="S22:W23"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="H16:I17"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="C33:H34"/>
-    <mergeCell ref="A38:J38"/>
-    <mergeCell ref="C30:H31"/>
-    <mergeCell ref="N22:R23"/>
+    <mergeCell ref="C33:I34"/>
     <mergeCell ref="A3:J6"/>
     <mergeCell ref="E12:F13"/>
     <mergeCell ref="B12:C13"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C24:D24"/>
     <mergeCell ref="H12:I13"/>
     <mergeCell ref="B7:I7"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="S22:W23"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="H16:I17"/>
+    <mergeCell ref="A38:J38"/>
+    <mergeCell ref="N22:R23"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C30:I31"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C24:D24" xr:uid="{107BE108-D45B-44D0-8B35-70F2F0EFD77C}">
-      <formula1>#REF!</formula1>
-    </dataValidation>
+    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C24" xr:uid="{107BE108-D45B-44D0-8B35-70F2F0EFD77C}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0" footer="0"/>

</xml_diff>